<commit_message>
Change the logic of goods Evaluate Analyse and Optimize the code of default search terms
</commit_message>
<xml_diff>
--- a/platform/service-boss/src/main/resources/download/goods_evaluate_analyse.xlsx
+++ b/platform/service-boss/src/main/resources/download/goods_evaluate_analyse.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgh\IdeaProjects\mall-shop\platform\service-boss\src\main\resources\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1497476-ECDB-4E41-B662-D9624822997A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B855C861-415E-4B9E-8B47-9FE0D6D54236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,46 +25,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>物流快</t>
+  </si>
+  <si>
+    <t>质量好</t>
+  </si>
+  <si>
+    <t>做工精致</t>
+  </si>
+  <si>
+    <t>很喜欢</t>
+  </si>
+  <si>
+    <t>很好</t>
+  </si>
+  <si>
+    <t>非常不错</t>
+  </si>
+  <si>
+    <t>非常棒</t>
+  </si>
+  <si>
+    <t>正版</t>
+  </si>
+  <si>
+    <t>味道不错</t>
+  </si>
+  <si>
+    <t>满意</t>
+  </si>
   <si>
     <t>evaluate_id</t>
-  </si>
-  <si>
-    <t>物流快</t>
-  </si>
-  <si>
-    <t>质量好</t>
-  </si>
-  <si>
-    <t>做工精致</t>
-  </si>
-  <si>
-    <t>很喜欢</t>
-  </si>
-  <si>
-    <t>很好</t>
-  </si>
-  <si>
-    <t>非常不错</t>
-  </si>
-  <si>
-    <t>非常棒</t>
-  </si>
-  <si>
-    <t>正版</t>
-  </si>
-  <si>
-    <t>味道不错</t>
-  </si>
-  <si>
-    <t>满意</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>evaluate_content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spu_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sku_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sku_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +91,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -100,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -382,51 +408,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>